<commit_message>
Cleaning up the Documentation
</commit_message>
<xml_diff>
--- a/Documentation/Key.xlsx
+++ b/Documentation/Key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s01bs8\Documents\grampian_data\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s01bs8\Documents\Scotland_Vulnerability_Resource\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE423164-5716-4E86-93EE-250FFC64F6D4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD822877-6D8D-4150-8708-52064B7BDADF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -483,18 +483,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -562,16 +556,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -583,19 +574,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -880,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A44" activeCellId="1" sqref="A42 A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.7265625" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
@@ -894,19 +888,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>134</v>
       </c>
     </row>
@@ -914,13 +908,13 @@
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>94</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>95</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -928,19 +922,19 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>97</v>
       </c>
     </row>
@@ -948,13 +942,13 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -962,19 +956,19 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>97</v>
       </c>
     </row>
@@ -982,13 +976,13 @@
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>132</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>133</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -996,19 +990,19 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="26" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1016,13 +1010,13 @@
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="4" t="s">
@@ -1030,19 +1024,19 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="26" x14ac:dyDescent="0.35">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1050,13 +1044,13 @@
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="4" t="s">
@@ -1064,19 +1058,19 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="26" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="9" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1084,13 +1078,13 @@
       <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E13" s="4" t="s">
@@ -1098,19 +1092,19 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="26" x14ac:dyDescent="0.35">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="9" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1118,13 +1112,13 @@
       <c r="A15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>33</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E15" s="4" t="s">
@@ -1132,19 +1126,19 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="39" x14ac:dyDescent="0.35">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1152,13 +1146,13 @@
       <c r="A17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>38</v>
       </c>
       <c r="E17" s="4" t="s">
@@ -1166,19 +1160,19 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="52" x14ac:dyDescent="0.35">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="9" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1186,13 +1180,13 @@
       <c r="A19" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>41</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E19" s="4" t="s">
@@ -1200,19 +1194,19 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="39" x14ac:dyDescent="0.35">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="9" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1220,13 +1214,13 @@
       <c r="A21" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="6" t="s">
         <v>47</v>
       </c>
       <c r="E21" s="4" t="s">
@@ -1234,19 +1228,19 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="26" x14ac:dyDescent="0.35">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="9" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1254,13 +1248,13 @@
       <c r="A23" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="6" t="s">
         <v>51</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="6" t="s">
         <v>52</v>
       </c>
       <c r="E23" s="4" t="s">
@@ -1268,19 +1262,19 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="52" x14ac:dyDescent="0.35">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="9" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1288,13 +1282,13 @@
       <c r="A25" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="6" t="s">
         <v>55</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="6" t="s">
         <v>56</v>
       </c>
       <c r="E25" s="4" t="s">
@@ -1302,19 +1296,19 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="39" x14ac:dyDescent="0.35">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="9" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1322,13 +1316,13 @@
       <c r="A27" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="6" t="s">
         <v>61</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="6" t="s">
         <v>62</v>
       </c>
       <c r="E27" s="4" t="s">
@@ -1336,19 +1330,19 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="39" x14ac:dyDescent="0.35">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="9" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1356,13 +1350,13 @@
       <c r="A29" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="6" t="s">
         <v>65</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="6" t="s">
         <v>66</v>
       </c>
       <c r="E29" s="4" t="s">
@@ -1370,19 +1364,19 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="39" x14ac:dyDescent="0.35">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D30" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E30" s="9" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1390,13 +1384,13 @@
       <c r="A31" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="6" t="s">
         <v>69</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="6" t="s">
         <v>70</v>
       </c>
       <c r="E31" s="4" t="s">
@@ -1404,19 +1398,19 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="39" x14ac:dyDescent="0.35">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="9" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1424,13 +1418,13 @@
       <c r="A33" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="6" t="s">
         <v>73</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="6" t="s">
         <v>74</v>
       </c>
       <c r="E33" s="4" t="s">
@@ -1438,19 +1432,19 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="39" x14ac:dyDescent="0.35">
-      <c r="A34" s="10" t="s">
+      <c r="A34" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="11" t="s">
+      <c r="D34" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="E34" s="9" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1458,13 +1452,13 @@
       <c r="A35" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="6" t="s">
         <v>77</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="6" t="s">
         <v>78</v>
       </c>
       <c r="E35" s="4" t="s">
@@ -1472,19 +1466,19 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="78" x14ac:dyDescent="0.35">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="D36" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E36" s="9" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1492,13 +1486,13 @@
       <c r="A37" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="6" t="s">
         <v>82</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="6" t="s">
         <v>84</v>
       </c>
       <c r="E37" s="4" t="s">
@@ -1506,19 +1500,19 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="39" x14ac:dyDescent="0.35">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D38" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="E38" s="9" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1526,13 +1520,13 @@
       <c r="A39" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="6" t="s">
         <v>89</v>
       </c>
       <c r="E39" s="4" t="s">
@@ -1540,19 +1534,19 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="39" x14ac:dyDescent="0.35">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C40" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D40" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="E40" s="9" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1560,13 +1554,13 @@
       <c r="A41" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="6" t="s">
         <v>92</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="6" t="s">
         <v>93</v>
       </c>
       <c r="E41" s="4" t="s">
@@ -1574,33 +1568,33 @@
       </c>
     </row>
     <row r="42" spans="1:5" ht="52" x14ac:dyDescent="0.35">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C42" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="D42" s="14" t="s">
+      <c r="D42" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="E42" s="10" t="s">
+      <c r="E42" s="9" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="52" x14ac:dyDescent="0.35">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="6" t="s">
         <v>101</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="D43" s="8" t="s">
         <v>102</v>
       </c>
       <c r="E43" s="4" t="s">
@@ -1608,33 +1602,33 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="52" x14ac:dyDescent="0.35">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="B44" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C44" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="D44" s="14" t="s">
+      <c r="D44" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="E44" s="9" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="52" x14ac:dyDescent="0.35">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="6" t="s">
         <v>105</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D45" s="9" t="s">
+      <c r="D45" s="8" t="s">
         <v>106</v>
       </c>
       <c r="E45" s="4" t="s">
@@ -1642,19 +1636,19 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="26" x14ac:dyDescent="0.35">
-      <c r="A46" s="10" t="s">
+      <c r="A46" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B46" s="11" t="s">
+      <c r="B46" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="D46" s="14" t="s">
+      <c r="D46" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="E46" s="10" t="s">
+      <c r="E46" s="9" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1662,13 +1656,13 @@
       <c r="A47" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="6" t="s">
         <v>109</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D47" s="9" t="s">
+      <c r="D47" s="8" t="s">
         <v>110</v>
       </c>
       <c r="E47" s="4" t="s">
@@ -1676,19 +1670,19 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="26" x14ac:dyDescent="0.35">
-      <c r="A48" s="10" t="s">
+      <c r="A48" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B48" s="11" t="s">
+      <c r="B48" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C48" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="D48" s="14" t="s">
+      <c r="D48" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="E48" s="10" t="s">
+      <c r="E48" s="9" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1696,13 +1690,13 @@
       <c r="A49" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="6" t="s">
         <v>113</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D49" s="9" t="s">
+      <c r="D49" s="8" t="s">
         <v>114</v>
       </c>
       <c r="E49" s="4" t="s">
@@ -1710,19 +1704,19 @@
       </c>
     </row>
     <row r="50" spans="1:5" ht="39" x14ac:dyDescent="0.35">
-      <c r="A50" s="10" t="s">
+      <c r="A50" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B50" s="11" t="s">
+      <c r="B50" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="C50" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="D50" s="14" t="s">
+      <c r="D50" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="E50" s="10" t="s">
+      <c r="E50" s="9" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1730,13 +1724,13 @@
       <c r="A51" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="6" t="s">
         <v>117</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D51" s="9" t="s">
+      <c r="D51" s="8" t="s">
         <v>118</v>
       </c>
       <c r="E51" s="4" t="s">
@@ -1744,33 +1738,33 @@
       </c>
     </row>
     <row r="52" spans="1:5" ht="26" x14ac:dyDescent="0.35">
-      <c r="A52" s="10" t="s">
+      <c r="A52" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B52" s="11" t="s">
+      <c r="B52" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="C52" s="10" t="s">
+      <c r="C52" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="D52" s="14" t="s">
+      <c r="D52" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="E52" s="10" t="s">
+      <c r="E52" s="9" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="39" x14ac:dyDescent="0.35">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="6" t="s">
         <v>121</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D53" s="9" t="s">
+      <c r="D53" s="8" t="s">
         <v>122</v>
       </c>
       <c r="E53" s="4" t="s">
@@ -1778,19 +1772,19 @@
       </c>
     </row>
     <row r="54" spans="1:5" ht="39" x14ac:dyDescent="0.35">
-      <c r="A54" s="6" t="s">
+      <c r="A54" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B54" s="11" t="s">
+      <c r="B54" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C54" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D54" s="14" t="s">
+      <c r="D54" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="E54" s="10" t="s">
+      <c r="E54" s="9" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>